<commit_message>
backend 99% complete, start on frontend
</commit_message>
<xml_diff>
--- a/dictionary.xlsx
+++ b/dictionary.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60aab64bfc0194a0/Documents/GitHub/ga-project-4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="8_{61371573-DD24-4BA1-BA9C-1B6FFA456F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A36ECBB-1AE1-4714-AFA0-A97F687C16BB}"/>
+  <xr:revisionPtr revIDLastSave="208" documentId="8_{61371573-DD24-4BA1-BA9C-1B6FFA456F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08F45C74-BFBE-4DB2-9387-32C76C4AA917}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1D9314D9-B417-4DA8-B094-1B82F4B65367}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{1D9314D9-B417-4DA8-B094-1B82F4B65367}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="endpoints" sheetId="2" r:id="rId2"/>
+    <sheet name="wireframe" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="98">
   <si>
     <t>frontend</t>
   </si>
@@ -568,13 +569,70 @@
   </si>
   <si>
     <t>/mod_log/new</t>
+  </si>
+  <si>
+    <t>app</t>
+  </si>
+  <si>
+    <t>homepage</t>
+  </si>
+  <si>
+    <t>users page</t>
+  </si>
+  <si>
+    <t>vendors page</t>
+  </si>
+  <si>
+    <t>featured products</t>
+  </si>
+  <si>
+    <t>profile page</t>
+  </si>
+  <si>
+    <t>on click show product page</t>
+  </si>
+  <si>
+    <t>buy button</t>
+  </si>
+  <si>
+    <t>=&gt; on click show shopping cart</t>
+  </si>
+  <si>
+    <t>order history</t>
+  </si>
+  <si>
+    <t>secondhand products on sale</t>
+  </si>
+  <si>
+    <t>inbox</t>
+  </si>
+  <si>
+    <t>not set up yet</t>
+  </si>
+  <si>
+    <t>might not want to show</t>
+  </si>
+  <si>
+    <t>moderator sign up</t>
+  </si>
+  <si>
+    <t>moderator login (modal)</t>
+  </si>
+  <si>
+    <t>register page(modal)</t>
+  </si>
+  <si>
+    <t>login page (modal)</t>
+  </si>
+  <si>
+    <t>wallets (modal)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -591,6 +649,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -631,7 +697,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -657,6 +723,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,6 +741,383 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>511680</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>56520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>571680</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>123480</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="2" name="Ink 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E326BFFE-02F6-DF8F-6DD6-1E65D73423C8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="1730880" y="1199520"/>
+            <a:ext cx="669600" cy="2352960"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Ink 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E326BFFE-02F6-DF8F-6DD6-1E65D73423C8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1724760" y="1193400"/>
+              <a:ext cx="681840" cy="2365200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>161880</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>162240</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76620</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="3" name="Ink 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEEAE3AB-729F-AB6E-FFF1-E03911275130}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2600280" y="3695760"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="3" name="Ink 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEEAE3AB-729F-AB6E-FFF1-E03911275130}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2594160" y="3689640"/>
+              <a:ext cx="12600" cy="12600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>171240</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>132060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57000</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>123120</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="4" name="Ink 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFAB456E-B958-CEE4-894C-2217D3D03AD1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2609640" y="3751560"/>
+            <a:ext cx="495360" cy="943560"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="4" name="Ink 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFAB456E-B958-CEE4-894C-2217D3D03AD1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2603520" y="3745440"/>
+              <a:ext cx="507600" cy="955800"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>399960</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>67920</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>26340</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="5" name="Ink 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00329A7F-2EBE-4A37-D7B5-4ED5E82D212D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="4057560" y="1428840"/>
+            <a:ext cx="277560" cy="693000"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="5" name="Ink 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00329A7F-2EBE-4A37-D7B5-4ED5E82D212D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4051440" y="1422720"/>
+              <a:ext cx="289800" cy="705240"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2023-09-07T06:17:20.836"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1860 81 24575,'-19'-1'0,"0"-1"0,-35-8 0,-6-2 0,-253-21 0,-464 11 0,733 24 0,-49 10 0,-37 2 0,126-15 0,0 1 0,-1 1 0,1-1 0,0 0 0,0 1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 1 0,0 0 0,0-1 0,1 1 0,-5 4 0,5-3 0,1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,1 0 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,1-1 0,-1 1 0,1 0 0,0 4 0,-1 72 0,4-1 0,3 1 0,18 85 0,1-7 0,21 91 0,-31-192 0,36 132 0,42 299 0,-54 16 0,-37-415 0,-4 1 0,-4-1 0,-29 144 0,31-216 0,-1 0 0,-1-1 0,-1 0 0,0-1 0,-1 1 0,-18 26 0,-4-3 0,-35 37 0,-14 16 0,69-79 0,-1 0 0,1 0 0,0 1 0,1 0 0,0 1 0,1 0 0,1 0 0,1 0 0,-8 25 0,2 23 0,3 0 0,-1 75 0,12 129 0,-2 34 0,-3-245 0,-3 0 0,-3 0 0,-19 73 0,16-77 0,3 1 0,2 1 0,2-1 0,3 1 0,5 64 0,-5 103 0,0-211 0,0-1 0,-1 0 0,1 0 0,-2 0 0,1 0 0,-1 0 0,-1-1 0,-7 13 0,6-11 0,0 0 0,0 1 0,2-1 0,-1 1 0,-4 16 0,3 20 0,2 1 0,2-1 0,1 1 0,9 61 0,2-8 0,7 137 0,-18 188 0,0-421 0,1 0 0,-1 1 0,1-1 0,-2 0 0,1 0 0,0 0 0,-1 0 0,-3 6 0,-3 10 0,8-18 0,1-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1 0,0-1 0,3 2 0,0 1 0,53 39 0,2-2 0,1-3 0,2-3 0,1-3 0,94 34 0,-144-62 0,0 1 0,0-2 0,1 0 0,0-1 0,-1 0 0,1-1 0,0-1 0,0 0 0,0-1 0,-1-1 0,1 0 0,0-1 0,-1-1 0,0 0 0,0-1 0,0 0 0,14-8 0,11 0 0,0 1 0,1 1 0,1 3 0,0 1 0,57-2 0,85-14 0,-164 18 0,-1-1 0,0-1 0,-1-1 0,19-9 0,-23 9 0,0 1 0,1 1 0,0 0 0,0 1 0,0 1 0,1 0 0,0 1 0,15-2 0,-12 5 0,-11 0 0,-1 1 0,1-1 0,0-1 0,0 1 0,-1-1 0,1-1 0,0 1 0,-1-1 0,1 0 0,-1 0 0,0-1 0,0 0 0,0 0 0,10-7 0,-15 9-33,-1 1 0,1-1-1,-1 0 1,1 0 0,-1 1-1,0-1 1,1 0 0,-1 0 0,0 0-1,0 1 1,0-1 0,1 0-1,-1 0 1,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,-1 0-1,1 0 1,0 1 0,0-1-1,0 0 1,-1 0 0,1 0-1,0 1 1,-1-1 0,1 0 0,-1 0-1,1 1 1,-1-1 0,1 1-1,-1-1 1,1 0 0,-1 1-1,0-1 1,1 1 0,-1-1 0,0 1-1,0-1 1,-11-7-6793</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2023-09-07T06:17:29.371"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0 24575,'0'0'-8191</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2023-09-07T06:18:31.972"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 30 24575,'-1'-1'0,"1"0"0,0 0 0,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,2 1 0,1-1 0,-1 0 0,0 1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,2 2 0,4 6 0,-1 0 0,0 1 0,-1 0 0,0 0 0,0 0 0,-1 1 0,-1 0 0,0 1 0,-1-1 0,0 1 0,-1-1 0,3 27 0,0 15 0,-3 97 0,-3-109 0,-4 1209 0,4-1190 0,2 1 0,4-1 0,2-1 0,3 1 0,2-1 0,26 70 0,11-17 0,-33-80 0,-2 1 0,-1 1 0,-2 1 0,15 68 0,-27-101 0,1 0 0,0 0 0,0 0 0,0 0 0,0-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,0 0 0,0 0 0,3 1 0,8 2 0,0 0 0,0-2 0,26 3 0,-26-4 0,59 3 0,-1-3 0,1-3 0,-1-4 0,0-2 0,133-34 0,-166 33 0,104-30 0,-125 32-455,1 2 0,28-5 0,-25 7-6371</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink4.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2023-09-07T06:20:33.338"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0 24575,'0'1101'0,"2"-1063"0,2 1 0,17 73 0,-12-73 0,-2 1 0,4 65 0,-13-9 0,0-55 0,1 0 0,6 45 0,-4-83 0,-1-1 0,1 1 0,0 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,5 1 0,4 2 0,1 0 0,1 0 0,17 3 0,-25-7 0,324 62 129,-99-23-1623,-184-31-5332</inkml:trace>
+</inkml:ink>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1123,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3F5953-C71B-4DA6-9D92-36CDD17DADFA}">
   <dimension ref="B2:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,4 +1822,109 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D706F10-0AA6-4495-B0E9-34ECBC1506B8}">
+  <dimension ref="E2:I26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="G2" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="G3" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E6" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E7" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E10" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E11" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="H14" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>